<commit_message>
Added Segment 2 Deliverables
</commit_message>
<xml_diff>
--- a/Project Tracker.xlsx
+++ b/Project Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yazhinigopal/Desktop/DAV Bootcamp/20 Final Project/Fake_News_Detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19A99D4-656A-1A47-984C-D3651C8E178C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8FC623-B0DF-914D-BD67-6C7E4229ADEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C0E8822A-E952-3943-A091-8C8A9793C91F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{C0E8822A-E952-3943-A091-8C8A9793C91F}"/>
   </bookViews>
   <sheets>
     <sheet name="Segment 1" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Segment 1'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Segment 2'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="67">
   <si>
     <t>Presentation</t>
   </si>
@@ -314,6 +315,201 @@
   </si>
   <si>
     <t>Action Items Tracker.xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">✓ Description of the data exploration phase of the project </t>
+  </si>
+  <si>
+    <t>✓ Description of the analysis phase of the project</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Main Branch - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All code necessary to perform exploratory analysis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Main Branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Some code necessary to complete the machine learning portion of the project </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>README.md</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Description of the communication protocols</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>README.md</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Outline of the project (this may include images, but should be easy to follow and digest)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Individual Branches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - At least one branch for each team member</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Individual Branches - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Each team member has at least four commits from the duration of the first segment</t>
+    </r>
+  </si>
+  <si>
+    <t>Description of preliminary data preprocessing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of preliminary feature engineering and preliminary feature selection, including their decision-making process </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of how data was split into training and testing sets </t>
+  </si>
+  <si>
+    <t>Explanation of model choice, including limitations and benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database stores static data for use during the project </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database interfaces with the project in some format (e.g., scraping updates the database, or database connects to the model) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes at least two tables </t>
+  </si>
+  <si>
+    <t>Provide your ERD with relationships for SQL Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storyboard on Google Slide(s) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes at least one join using the database language (not including any joins in Pandas) </t>
+  </si>
+  <si>
+    <t>Includes at least one connection string using SQLAlchemy</t>
+  </si>
+  <si>
+    <t>Raza</t>
+  </si>
+  <si>
+    <t>Raza/Yaz</t>
+  </si>
+  <si>
+    <t>Shruti</t>
+  </si>
+  <si>
+    <t>Nida/Shruti</t>
+  </si>
+  <si>
+    <t>Description of the tool(s) that will be used to create final dashboard (Tableau, Flask, HTML, CSS)</t>
+  </si>
+  <si>
+    <t>Description of interactive element(s) (Tableau reports with cross filters &amp; FakeNewsDetection webpage)</t>
   </si>
 </sst>
 </file>
@@ -410,7 +606,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -694,11 +890,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -805,6 +1066,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -829,32 +1117,65 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC6A791-3EFA-2F40-BB84-73C8821E3B02}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="116" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1209,10 +1530,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -1223,8 +1544,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40"/>
-      <c r="B3" s="49" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="41" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1235,8 +1556,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="49" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="41" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1247,8 +1568,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="50" t="s">
+      <c r="A5" s="50"/>
+      <c r="B5" s="42" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1259,7 +1580,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="45" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1274,7 +1595,7 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="14" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1608,7 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
@@ -1300,7 +1621,7 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
@@ -1313,7 +1634,7 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="45" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1328,7 +1649,7 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
@@ -1341,7 +1662,7 @@
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="43"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="24" t="s">
         <v>34</v>
       </c>
@@ -1354,7 +1675,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="43"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="33" t="s">
         <v>24</v>
       </c>
@@ -1367,7 +1688,7 @@
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="15" t="s">
         <v>29</v>
       </c>
@@ -1380,7 +1701,7 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="45" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -1395,7 +1716,7 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="34" t="s">
         <v>30</v>
       </c>
@@ -1408,7 +1729,7 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="17" t="s">
         <v>31</v>
       </c>
@@ -1421,23 +1742,23 @@
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="47" t="s">
+      <c r="C18" s="38"/>
+      <c r="D18" s="39" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="43" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="23" t="s">
@@ -1449,8 +1770,8 @@
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="52" t="s">
+      <c r="A20" s="50"/>
+      <c r="B20" s="44" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -1511,12 +1832,456 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BEFF3A-D715-F249-BD13-CDFC75D8D16D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="49"/>
+      <c r="B3" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="49"/>
+      <c r="B4" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="53"/>
+      <c r="B5" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="53"/>
+      <c r="B6" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
+      <c r="B7" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="57"/>
+      <c r="B9" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="46"/>
+      <c r="B10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="46"/>
+      <c r="B11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="46"/>
+      <c r="B12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="46"/>
+      <c r="B15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="52"/>
+      <c r="B16" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="52"/>
+      <c r="B17" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="52"/>
+      <c r="B18" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="52"/>
+      <c r="B19" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52"/>
+      <c r="B20" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="51"/>
+      <c r="B22" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="51"/>
+      <c r="B23" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="51"/>
+      <c r="B24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="47"/>
+      <c r="B25" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="51"/>
+      <c r="B27" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="63"/>
+      <c r="B28" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="50"/>
+      <c r="B30" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{A934AC89-630D-7B47-AB83-0067BB1BB5A3}"/>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A26:A28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>